<commit_message>
✨ Enhance process_repositories method to handle missing topic values and report most common topics
</commit_message>
<xml_diff>
--- a/repos.xlsx
+++ b/repos.xlsx
@@ -18568,12 +18568,12 @@
       </c>
       <c r="AW52" t="inlineStr">
         <is>
-          <t>2025-01-02T05:37:31Z</t>
+          <t>2025-01-02T06:11:07Z</t>
         </is>
       </c>
       <c r="AX52" t="inlineStr">
         <is>
-          <t>2025-01-02T05:37:28Z</t>
+          <t>2025-01-02T06:11:03Z</t>
         </is>
       </c>
       <c r="AY52" t="inlineStr">

</xml_diff>